<commit_message>
Kosten näher betrachtet und Struktur bei 9_1_2 angelegt
</commit_message>
<xml_diff>
--- a/9_2_VLT_Variation/FBH_Preisvariation/9_2_Kosten_FBH_PReis.xlsx
+++ b/9_2_VLT_Variation/FBH_Preisvariation/9_2_Kosten_FBH_PReis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fraunhofer-my.sharepoint.com/personal/lara_josephine_barnic_iee_fraunhofer_de/Documents/A_Bearbeitung/9_Parameterstudie_REP/9_2_VLT_Variation/FBH_Preisvariation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1315" documentId="11_AD4DB114E441178AC67DF4879E90C19A693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2894FAEB-555D-402A-935F-DF61A5678DA3}"/>
+  <xr:revisionPtr revIDLastSave="1316" documentId="11_AD4DB114E441178AC67DF4879E90C19A693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B03A5DD7-C105-4931-937F-705BF8B5C478}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-140" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -302,7 +302,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A10763E-D0ED-4F3F-86F0-CEDFE4EEB962}" type="CELLRANGE">
+                    <a:fld id="{269429C9-9933-4506-A7EC-798FB59A1CEA}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -336,7 +336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15869652-AE0D-44D6-96AE-08710AC7F8EF}" type="CELLRANGE">
+                    <a:fld id="{11F06730-8221-4F95-B47F-C4B2E09A4F50}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1176,7 +1176,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E5EC617-00EC-4E6C-82CA-2B76983B087C}" type="CELLRANGE">
+                    <a:fld id="{4E020BF4-551A-4FB5-8D5F-D2B81B845A33}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1209,7 +1209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E75541D4-4861-4265-9A8D-D34BFCC95764}" type="CELLRANGE">
+                    <a:fld id="{D4093465-BE23-4A55-91BF-9804E79FE8AC}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -2965,7 +2965,7 @@
       <sheetName val="kalte NW"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="3">
           <cell r="K3">
             <v>2.7262505862299999</v>
@@ -2991,10 +2991,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3047,10 +3047,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3318,24 +3314,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5395E545-C7E4-4937-89EC-C03939104281}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3349,7 +3345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F3" s="2"/>
       <c r="J3" s="1" t="s">
         <v>0</v>
@@ -3371,7 +3367,7 @@
         <v>0.42056058079468261</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -3391,7 +3387,7 @@
         <v>344.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" cm="1">
         <f t="array" ref="A5:E8">[1]Zusammenfassung!$J$2:$N$5</f>
         <v>0</v>
@@ -3428,7 +3424,7 @@
         <v>0.50272456861868342</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <v>dezentral</v>
       </c>
@@ -3445,7 +3441,7 @@
         <v>0.20775715438043485</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <v>NT-WN</v>
       </c>
@@ -3465,7 +3461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <v>kalte NW</v>
       </c>
@@ -3482,7 +3478,7 @@
         <v>0.29088426284972324</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3494,7 +3490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3511,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -3535,7 +3531,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -3555,7 +3551,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
@@ -3563,7 +3559,7 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3577,7 +3573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -3597,7 +3593,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -3616,7 +3612,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -3635,22 +3631,22 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J30" t="s">
         <v>8</v>
       </c>

</xml_diff>